<commit_message>
Diagrama de normalizacion creado
</commit_message>
<xml_diff>
--- a/EjercicioUniversidad/EjercicioUniversidad.xlsx
+++ b/EjercicioUniversidad/EjercicioUniversidad.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t>Universidad</t>
   </si>
@@ -27,18 +27,6 @@
     <t>Facultad</t>
   </si>
   <si>
-    <t>Escuelas</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Director</t>
-  </si>
-  <si>
-    <t>Decano</t>
-  </si>
-  <si>
     <t>Dirección exacta</t>
   </si>
   <si>
@@ -48,12 +36,6 @@
     <t>Sede regional</t>
   </si>
   <si>
-    <t>Región a la que pertenece</t>
-  </si>
-  <si>
-    <t>Facultad a la que  pertenece</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ubicación exacta </t>
   </si>
   <si>
@@ -63,9 +45,6 @@
     <t>Grado</t>
   </si>
   <si>
-    <t>Escuela o sede a la que pertenece</t>
-  </si>
-  <si>
     <t>Donde se imparte</t>
   </si>
   <si>
@@ -87,9 +66,6 @@
     <t>Curso</t>
   </si>
   <si>
-    <t>Sigla</t>
-  </si>
-  <si>
     <t>Requisitos</t>
   </si>
   <si>
@@ -105,18 +81,9 @@
     <t>Grado academico</t>
   </si>
   <si>
-    <t>Do-requisitos</t>
-  </si>
-  <si>
-    <t>Emails</t>
-  </si>
-  <si>
     <t>Teléfono</t>
   </si>
   <si>
-    <t>Decano/Director</t>
-  </si>
-  <si>
     <t>Estudiante</t>
   </si>
   <si>
@@ -126,17 +93,149 @@
     <t>Apellidos</t>
   </si>
   <si>
-    <t># de carnet</t>
-  </si>
-  <si>
-    <t>Fecha de ingreso a la Universidad</t>
+    <t>nota</t>
+  </si>
+  <si>
+    <t>condicion</t>
+  </si>
+  <si>
+    <t>Co-requisitos</t>
+  </si>
+  <si>
+    <t>Escuela</t>
+  </si>
+  <si>
+    <t>Nombre sede</t>
+  </si>
+  <si>
+    <t>Nombre carrera</t>
+  </si>
+  <si>
+    <t>Nombre curso</t>
+  </si>
+  <si>
+    <t>Nombre estudiante</t>
+  </si>
+  <si>
+    <t>Nombre escuela</t>
+  </si>
+  <si>
+    <t>Nombre facultad</t>
+  </si>
+  <si>
+    <t>Facultad a la que pertenece</t>
+  </si>
+  <si>
+    <t>Fecha de ingreso a la U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escuela o sede de pertenencia </t>
+  </si>
+  <si>
+    <t>Director/decano</t>
+  </si>
+  <si>
+    <t>Región</t>
+  </si>
+  <si>
+    <t>Sigla de curso</t>
+  </si>
+  <si>
+    <t>Fecha de matrícula</t>
+  </si>
+  <si>
+    <t>Ubicación facultad</t>
+  </si>
+  <si>
+    <t>ID facultad</t>
+  </si>
+  <si>
+    <t>Director/Decano escuela</t>
+  </si>
+  <si>
+    <t>Director/Decano facultad</t>
+  </si>
+  <si>
+    <t>Director/Decano sede</t>
+  </si>
+  <si>
+    <t>ID sede</t>
+  </si>
+  <si>
+    <t>Escuela o sede de pertenencia</t>
+  </si>
+  <si>
+    <t>ID carrera</t>
+  </si>
+  <si>
+    <t>Fecha de matricula</t>
+  </si>
+  <si>
+    <t>Nombre de  curso</t>
+  </si>
+  <si>
+    <t>Siglas de curso</t>
+  </si>
+  <si>
+    <t>Nombre Director/decano</t>
+  </si>
+  <si>
+    <t>Cédula Director/decano</t>
+  </si>
+  <si>
+    <t>Grado académico</t>
+  </si>
+  <si>
+    <t>Ponderado carrera</t>
+  </si>
+  <si>
+    <t>Telefono(multi)</t>
+  </si>
+  <si>
+    <t>Email(multi)</t>
+  </si>
+  <si>
+    <t>ID escuela</t>
+  </si>
+  <si>
+    <t>Región sede</t>
+  </si>
+  <si>
+    <t>Apellidos estudiante</t>
+  </si>
+  <si>
+    <t>Cédula estudiante</t>
+  </si>
+  <si>
+    <t>Fecha nacimiento</t>
+  </si>
+  <si>
+    <t>Fecha de ingreso</t>
+  </si>
+  <si>
+    <t># carnet estudiante</t>
+  </si>
+  <si>
+    <t># de carnet estudiante</t>
+  </si>
+  <si>
+    <t>cantidad de attrs</t>
+  </si>
+  <si>
+    <t>Nota curso</t>
+  </si>
+  <si>
+    <t>Ponderado estudiante</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,19 +250,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.749992370372631"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -183,8 +282,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -240,27 +375,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,235 +764,593 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="5">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B11" s="5">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="G11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+      <c r="C13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+      <c r="C14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
+      <c r="C15" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="24"/>
+      <c r="C17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="24"/>
+      <c r="C18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="23"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
+      <c r="C19" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="23"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="24"/>
+      <c r="C20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="23"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="20"/>
+      <c r="C21" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="20"/>
+      <c r="C22" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="20"/>
+      <c r="C23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="20"/>
+      <c r="C24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="19"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="17"/>
+      <c r="C25" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="17"/>
+      <c r="C26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="18"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="17"/>
+      <c r="C27" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="18"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="17"/>
+      <c r="C28" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="18"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="17"/>
+      <c r="C29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="18"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="17"/>
+      <c r="C30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="17"/>
+      <c r="C31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="22"/>
+      <c r="C32" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="21"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="22"/>
+      <c r="C33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="21"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="22"/>
+      <c r="C34" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="21"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="22"/>
+      <c r="C35" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="21"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="22"/>
+      <c r="C36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="21"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="17"/>
+      <c r="C37" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="18"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="17"/>
+      <c r="C38" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="18"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="20"/>
+      <c r="C39" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="19"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="20"/>
+      <c r="C40" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="19"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="20"/>
+      <c r="C41" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="19"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="20"/>
+      <c r="C42" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="19"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="20"/>
+      <c r="C43" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="19"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="20"/>
+      <c r="C44" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="19"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="20"/>
+      <c r="C45" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="19"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="17"/>
+      <c r="C46" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="D46" s="18"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="17"/>
+      <c r="C47" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="18"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="17"/>
+      <c r="C48" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="18"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="17"/>
+      <c r="C49" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="18"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="17"/>
+      <c r="C50" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="18"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="17"/>
+      <c r="C51" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+  <mergeCells count="17">
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="B46:B51"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="D46:D51"/>
+    <mergeCell ref="D39:D45"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="D17:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>